<commit_message>
Position and maximum in treated images
</commit_message>
<xml_diff>
--- a/Positions_vis.xlsx
+++ b/Positions_vis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gérémy\Documents\GitHub\Optique_experimentale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46370CB2-CD75-417E-87BA-53BE26F22357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CE29E5-410F-40C5-AEBE-670C0DDB93C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{8B30FCDA-6F0D-4095-BE06-B9C0189DC30A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{8B30FCDA-6F0D-4095-BE06-B9C0189DC30A}"/>
   </bookViews>
   <sheets>
     <sheet name="HeNe" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Vitamin Water</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>4.0 saccharose</t>
+  </si>
+  <si>
+    <t>2.8 saccharose</t>
   </si>
 </sst>
 </file>
@@ -467,9 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E379113-D58C-411B-9368-75E0B518F771}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -480,7 +481,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -615,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3379AC-FAEA-40E2-B4FD-5127EDE91E90}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changing name of measures
</commit_message>
<xml_diff>
--- a/Positions_vis.xlsx
+++ b/Positions_vis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gérémy\Documents\GitHub\Optique_experimentale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CE29E5-410F-40C5-AEBE-670C0DDB93C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE145F5B-616B-462B-A7DD-4B4F9F887EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{8B30FCDA-6F0D-4095-BE06-B9C0189DC30A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{8B30FCDA-6F0D-4095-BE06-B9C0189DC30A}"/>
   </bookViews>
   <sheets>
     <sheet name="HeNe" sheetId="1" r:id="rId1"/>
@@ -48,18 +48,9 @@
     <t>Gatorade</t>
   </si>
   <si>
-    <t>Ethanol</t>
-  </si>
-  <si>
-    <t>Acetone</t>
-  </si>
-  <si>
     <t>2.5 saccharose</t>
   </si>
   <si>
-    <t>Gatorade zero</t>
-  </si>
-  <si>
     <t>3.0 saccharose</t>
   </si>
   <si>
@@ -72,9 +63,6 @@
     <t>5.0 saccharose</t>
   </si>
   <si>
-    <t>Water</t>
-  </si>
-  <si>
     <t>3.5 saccharose</t>
   </si>
   <si>
@@ -82,6 +70,18 @@
   </si>
   <si>
     <t>2.8 saccharose</t>
+  </si>
+  <si>
+    <t>Gatorade zéro</t>
+  </si>
+  <si>
+    <t>Éthanol</t>
+  </si>
+  <si>
+    <t>Eau</t>
+  </si>
+  <si>
+    <t>Acétone</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E379113-D58C-411B-9368-75E0B518F771}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -481,40 +483,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -616,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3379AC-FAEA-40E2-B4FD-5127EDE91E90}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,43 +629,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>